<commit_message>
minor fixes and parametrization
</commit_message>
<xml_diff>
--- a/02_parameter/02_diccionario_coaliciones/diccionario_siglacoa_v2.xlsx
+++ b/02_parameter/02_diccionario_coaliciones/diccionario_siglacoa_v2.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\goyan\Desktop\Simulador_electoral\02_parameter\02_diccionario_coaliciones\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{9C163C5D-AA89-44E3-9413-2242124AF63D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF69F151-5F83-4A95-B7A3-7EA64693B3E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="diccionario_siglacoa_v2" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="84">
   <si>
     <t>Sigla</t>
   </si>
@@ -245,12 +245,39 @@
   </si>
   <si>
     <t>JAK</t>
+  </si>
+  <si>
+    <t>IzquierdaDiv</t>
+  </si>
+  <si>
+    <t>DC-IC-CIU</t>
+  </si>
+  <si>
+    <t>Progresistas</t>
+  </si>
+  <si>
+    <t>Realista</t>
+  </si>
+  <si>
+    <t>Chile Digno</t>
+  </si>
+  <si>
+    <t>Unidad Constituyente</t>
+  </si>
+  <si>
+    <t>Humanista</t>
+  </si>
+  <si>
+    <t>D2020</t>
+  </si>
+  <si>
+    <t>UC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -728,8 +755,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1084,16 +1112,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:O29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="P27" sqref="P27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1130,8 +1158,17 @@
       <c r="L1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M1" t="s">
+        <v>75</v>
+      </c>
+      <c r="N1" t="s">
+        <v>78</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1168,8 +1205,17 @@
       <c r="L2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -1206,8 +1252,17 @@
       <c r="L3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M3" t="s">
+        <v>13</v>
+      </c>
+      <c r="N3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -1244,8 +1299,17 @@
       <c r="L4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N4" t="s">
+        <v>13</v>
+      </c>
+      <c r="O4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -1282,8 +1346,17 @@
       <c r="L5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M5" t="s">
+        <v>76</v>
+      </c>
+      <c r="N5" t="s">
+        <v>80</v>
+      </c>
+      <c r="O5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -1320,8 +1393,17 @@
       <c r="L6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M6" t="s">
+        <v>13</v>
+      </c>
+      <c r="N6" t="s">
+        <v>13</v>
+      </c>
+      <c r="O6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -1358,8 +1440,17 @@
       <c r="L7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M7" t="s">
+        <v>13</v>
+      </c>
+      <c r="N7" t="s">
+        <v>13</v>
+      </c>
+      <c r="O7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -1396,8 +1487,17 @@
       <c r="L8" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M8" t="s">
+        <v>16</v>
+      </c>
+      <c r="N8" t="s">
+        <v>16</v>
+      </c>
+      <c r="O8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -1434,8 +1534,17 @@
       <c r="L9" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M9" t="s">
+        <v>34</v>
+      </c>
+      <c r="N9" t="s">
+        <v>81</v>
+      </c>
+      <c r="O9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>35</v>
       </c>
@@ -1472,8 +1581,17 @@
       <c r="L10" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M10" t="s">
+        <v>77</v>
+      </c>
+      <c r="N10" t="s">
+        <v>80</v>
+      </c>
+      <c r="O10" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>37</v>
       </c>
@@ -1510,8 +1628,17 @@
       <c r="L11" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M11" t="s">
+        <v>34</v>
+      </c>
+      <c r="N11" t="s">
+        <v>79</v>
+      </c>
+      <c r="O11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -1548,8 +1675,17 @@
       <c r="L12" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M12" t="s">
+        <v>34</v>
+      </c>
+      <c r="N12" t="s">
+        <v>79</v>
+      </c>
+      <c r="O12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>40</v>
       </c>
@@ -1586,8 +1722,17 @@
       <c r="L13" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M13" t="s">
+        <v>41</v>
+      </c>
+      <c r="N13" t="s">
+        <v>31</v>
+      </c>
+      <c r="O13" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>42</v>
       </c>
@@ -1624,8 +1769,17 @@
       <c r="L14" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M14" t="s">
+        <v>41</v>
+      </c>
+      <c r="N14" t="s">
+        <v>31</v>
+      </c>
+      <c r="O14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>43</v>
       </c>
@@ -1662,8 +1816,17 @@
       <c r="L15" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M15" t="s">
+        <v>41</v>
+      </c>
+      <c r="N15" t="s">
+        <v>79</v>
+      </c>
+      <c r="O15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>44</v>
       </c>
@@ -1700,8 +1863,17 @@
       <c r="L16" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M16" t="s">
+        <v>41</v>
+      </c>
+      <c r="N16" t="s">
+        <v>31</v>
+      </c>
+      <c r="O16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>45</v>
       </c>
@@ -1738,8 +1910,17 @@
       <c r="L17" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M17" t="s">
+        <v>46</v>
+      </c>
+      <c r="N17" t="s">
+        <v>46</v>
+      </c>
+      <c r="O17" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>48</v>
       </c>
@@ -1776,8 +1957,17 @@
       <c r="L18" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M18" t="s">
+        <v>50</v>
+      </c>
+      <c r="N18" t="s">
+        <v>79</v>
+      </c>
+      <c r="O18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>51</v>
       </c>
@@ -1814,8 +2004,17 @@
       <c r="L19" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M19" t="s">
+        <v>50</v>
+      </c>
+      <c r="N19" t="s">
+        <v>79</v>
+      </c>
+      <c r="O19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>52</v>
       </c>
@@ -1852,8 +2051,17 @@
       <c r="L20" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M20" t="s">
+        <v>54</v>
+      </c>
+      <c r="N20" t="s">
+        <v>54</v>
+      </c>
+      <c r="O20" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>55</v>
       </c>
@@ -1890,8 +2098,17 @@
       <c r="L21" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M21" t="s">
+        <v>54</v>
+      </c>
+      <c r="N21" t="s">
+        <v>54</v>
+      </c>
+      <c r="O21" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>57</v>
       </c>
@@ -1928,8 +2145,17 @@
       <c r="L22" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M22" t="s">
+        <v>41</v>
+      </c>
+      <c r="N22" t="s">
+        <v>79</v>
+      </c>
+      <c r="O22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>61</v>
       </c>
@@ -1966,8 +2192,17 @@
       <c r="L23" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M23" t="s">
+        <v>41</v>
+      </c>
+      <c r="N23" t="s">
+        <v>79</v>
+      </c>
+      <c r="O23" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>63</v>
       </c>
@@ -2004,8 +2239,17 @@
       <c r="L24" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M24" t="s">
+        <v>76</v>
+      </c>
+      <c r="N24" t="s">
+        <v>80</v>
+      </c>
+      <c r="O24" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>66</v>
       </c>
@@ -2042,8 +2286,17 @@
       <c r="L25" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M25" t="s">
+        <v>77</v>
+      </c>
+      <c r="N25" t="s">
+        <v>80</v>
+      </c>
+      <c r="O25" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>68</v>
       </c>
@@ -2080,8 +2333,17 @@
       <c r="L26" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M26" t="s">
+        <v>77</v>
+      </c>
+      <c r="N26" t="s">
+        <v>80</v>
+      </c>
+      <c r="O26" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>69</v>
       </c>
@@ -2118,8 +2380,17 @@
       <c r="L27" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M27" t="s">
+        <v>76</v>
+      </c>
+      <c r="N27" t="s">
+        <v>80</v>
+      </c>
+      <c r="O27" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>70</v>
       </c>
@@ -2156,8 +2427,17 @@
       <c r="L28" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M28" t="s">
+        <v>77</v>
+      </c>
+      <c r="N28" t="s">
+        <v>80</v>
+      </c>
+      <c r="O28" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>71</v>
       </c>
@@ -2192,6 +2472,15 @@
         <v>27</v>
       </c>
       <c r="L29" t="s">
+        <v>74</v>
+      </c>
+      <c r="M29" t="s">
+        <v>13</v>
+      </c>
+      <c r="N29" t="s">
+        <v>74</v>
+      </c>
+      <c r="O29" t="s">
         <v>74</v>
       </c>
     </row>

</xml_diff>

<commit_message>
more complexity and code cleaning
</commit_message>
<xml_diff>
--- a/02_parameter/02_diccionario_coaliciones/diccionario_siglacoa_v2.xlsx
+++ b/02_parameter/02_diccionario_coaliciones/diccionario_siglacoa_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\goyan\Desktop\Simulador_electoral\02_parameter\02_diccionario_coaliciones\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF69F151-5F83-4A95-B7A3-7EA64693B3E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62001D49-134A-4AA6-900D-FB1E911B78F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1115,8 +1115,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="P27" sqref="P27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O30" sqref="O30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2481,7 +2481,7 @@
         <v>74</v>
       </c>
       <c r="O29" t="s">
-        <v>74</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>